<commit_message>
Cambio de estructura de archivos
</commit_message>
<xml_diff>
--- a/Facturas/Factura 1.xlsx
+++ b/Facturas/Factura 1.xlsx
@@ -815,13 +815,13 @@
         </is>
       </c>
       <c r="E5" s="24" t="n">
-        <v>9.199999999999999</v>
+        <v>9</v>
       </c>
       <c r="F5" s="9" t="n">
         <v>250</v>
       </c>
       <c r="G5" s="11" t="n">
-        <v>2300</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="6" ht="24.95" customHeight="1">
@@ -839,13 +839,13 @@
         </is>
       </c>
       <c r="E6" s="24" t="n">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="F6" s="9" t="n">
         <v>25</v>
       </c>
       <c r="G6" s="11" t="n">
-        <v>2750</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="7" ht="24.95" customHeight="1">

</xml_diff>